<commit_message>
Added message conformance resources
Refined Profile and Terminology page wording. Adjusted certain resource names to increase consistency. Added responder CapabilityStatement, request and response MessageHeader and Bundle definitions.
</commit_message>
<xml_diff>
--- a/output/carin-rtpbc-MedicationRequest.xlsx
+++ b/output/carin-rtpbc-MedicationRequest.xlsx
@@ -824,7 +824,7 @@
     <t>Patient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/carin/StructureDefinition/rtpbc-request-patient-info)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/carin/StructureDefinition/rtpbc-patient)
 </t>
   </si>
   <si>
@@ -1015,7 +1015,7 @@
     <t>Prescriber</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/carin/StructureDefinition/rtpbc-request-prescriber-info)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/carin/StructureDefinition/rtpbc-practitioner)
 </t>
   </si>
   <si>

</xml_diff>